<commit_message>
edit l_double -print on treeview issue
</commit_message>
<xml_diff>
--- a/xl/test.xlsx
+++ b/xl/test.xlsx
@@ -434,7 +434,7 @@
         <v>780</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -457,7 +457,9 @@
       <c r="B8" s="4" t="n">
         <v>1000</v>
       </c>
-      <c r="C8" s="3" t="n"/>
+      <c r="C8" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
@@ -570,7 +572,9 @@
       <c r="B3" s="4" t="n">
         <v>1000</v>
       </c>
-      <c r="C3" s="3" t="n"/>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
@@ -593,7 +597,7 @@
         <v>2000</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -674,6 +678,9 @@
       <c r="B2" s="4" t="n">
         <v>1000</v>
       </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
@@ -723,6 +730,9 @@
       </c>
       <c r="B7" s="4" t="n">
         <v>930</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -823,6 +833,9 @@
       <c r="B3" s="4" t="n">
         <v>930</v>
       </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="8">
       <c r="A4" s="4" t="inlineStr">
@@ -853,6 +866,9 @@
       <c r="B6" s="4" t="n">
         <v>1200</v>
       </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="8">
       <c r="A7" s="4" t="inlineStr">
@@ -864,7 +880,7 @@
         <v>6000</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="8">
@@ -875,6 +891,9 @@
       </c>
       <c r="B8" s="4" t="n">
         <v>1000</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="8">
@@ -2027,7 +2046,7 @@
         <v>2600</v>
       </c>
       <c r="C6" s="7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1" s="8">
@@ -2040,7 +2059,7 @@
         <v>3000</v>
       </c>
       <c r="C7" s="7" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="8">
@@ -2053,7 +2072,7 @@
         <v>3000</v>
       </c>
       <c r="C8" s="7" t="n">
-        <v>65</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="8">
@@ -2066,7 +2085,7 @@
         <v>2000</v>
       </c>
       <c r="C9" s="7" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1" s="8">
@@ -2079,7 +2098,7 @@
         <v>2500</v>
       </c>
       <c r="C10" s="7" t="n">
-        <v>234</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1" s="8">
@@ -2105,7 +2124,7 @@
         <v>9000</v>
       </c>
       <c r="C12" s="7" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1" s="8">
@@ -2118,7 +2137,7 @@
         <v>8000</v>
       </c>
       <c r="C13" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1" s="8">

</xml_diff>

<commit_message>
fix print treeview issue
</commit_message>
<xml_diff>
--- a/xl/test.xlsx
+++ b/xl/test.xlsx
@@ -446,7 +446,9 @@
       <c r="B7" s="4" t="n">
         <v>1100</v>
       </c>
-      <c r="C7" s="3" t="n"/>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
@@ -561,7 +563,9 @@
       <c r="B2" s="4" t="n">
         <v>1100</v>
       </c>
-      <c r="C2" s="3" t="n"/>
+      <c r="C2" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
@@ -2059,7 +2063,7 @@
         <v>3000</v>
       </c>
       <c r="C7" s="7" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="8">
@@ -2072,7 +2076,7 @@
         <v>3000</v>
       </c>
       <c r="C8" s="7" t="n">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="8">
@@ -2098,7 +2102,7 @@
         <v>2500</v>
       </c>
       <c r="C10" s="7" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1" s="8">
@@ -2111,7 +2115,7 @@
         <v>2000</v>
       </c>
       <c r="C11" s="7" t="n">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1" s="8">

</xml_diff>

<commit_message>
add save on personal.xl
</commit_message>
<xml_diff>
--- a/xl/test.xlsx
+++ b/xl/test.xlsx
@@ -930,7 +930,7 @@
         <v>4000</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1" s="8">
@@ -1960,7 +1960,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1998,7 +1998,7 @@
         <v>8000</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="8">
@@ -2011,7 +2011,7 @@
         <v>8000</v>
       </c>
       <c r="C3" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="8">
@@ -2024,7 +2024,7 @@
         <v>2400</v>
       </c>
       <c r="C4" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="8">
@@ -2037,7 +2037,7 @@
         <v>2600</v>
       </c>
       <c r="C5" s="7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="8">
@@ -2063,7 +2063,7 @@
         <v>3000</v>
       </c>
       <c r="C7" s="7" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1" s="8">
@@ -2076,7 +2076,7 @@
         <v>3000</v>
       </c>
       <c r="C8" s="7" t="n">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1" s="8">
@@ -2102,7 +2102,7 @@
         <v>2500</v>
       </c>
       <c r="C10" s="7" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1" s="8">
@@ -2115,7 +2115,7 @@
         <v>2000</v>
       </c>
       <c r="C11" s="7" t="n">
-        <v>37</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1" s="8">
@@ -2154,7 +2154,7 @@
         <v>9000</v>
       </c>
       <c r="C14" s="7" t="n">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1" s="8"/>

</xml_diff>